<commit_message>
Prepare for new release with fix for R4.x.x
</commit_message>
<xml_diff>
--- a/tests/testthat/hidden.xlsx
+++ b/tests/testthat/hidden.xlsx
@@ -1,26 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demin\Documents\yadisk\WindowsSync\excel.link\tests\testthat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cekor\Documents\excel.link\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DB3E32D-1BB5-4FA8-ABDB-335F1FB814B5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2C6ABCE-D247-403C-B6BC-22356D8E091B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17235" windowHeight="6585" activeTab="2" xr2:uid="{85319D3E-BC09-45BF-B3DC-783806C1E433}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{DB106540-66A3-402B-A80B-06A64576FE65}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="iris" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="cars" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -858,26 +867,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4933600-6D15-4DBD-BCE6-D076D3E808B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D65EB2-FE4C-4275-A81F-273A9469D424}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCD3611-F962-487B-954A-C43B0BFF9188}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29CDA24-6CB3-4CD5-9499-38524AAE6B30}">
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -894,7 +903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -914,7 +923,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -934,7 +943,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -954,7 +963,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -974,7 +983,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -994,7 +1003,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1014,7 +1023,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1034,7 +1043,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1054,7 +1063,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1074,7 +1083,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1094,7 +1103,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1114,7 +1123,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1134,7 +1143,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1154,7 +1163,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1174,7 +1183,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1194,7 +1203,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1214,7 +1223,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1234,7 +1243,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1254,7 +1263,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1274,7 +1283,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1294,7 +1303,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1314,7 +1323,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1334,7 +1343,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1354,7 +1363,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1374,7 +1383,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1394,7 +1403,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1414,7 +1423,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1434,7 +1443,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1454,7 +1463,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1474,7 +1483,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1494,7 +1503,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1514,7 +1523,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1534,7 +1543,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1554,7 +1563,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1574,7 +1583,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1594,7 +1603,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1614,7 +1623,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1634,7 +1643,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1654,7 +1663,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1674,7 +1683,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -1694,7 +1703,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1714,7 +1723,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -1734,7 +1743,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1754,7 +1763,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -1774,7 +1783,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1794,7 +1803,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -1814,7 +1823,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -1834,7 +1843,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1854,7 +1863,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -1874,7 +1883,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -1894,7 +1903,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -1914,7 +1923,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -1934,7 +1943,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -1954,7 +1963,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -1974,7 +1983,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -1994,7 +2003,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -2014,7 +2023,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -2034,7 +2043,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -2054,7 +2063,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -2074,7 +2083,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -2094,7 +2103,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -2114,7 +2123,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>66</v>
       </c>
@@ -2134,7 +2143,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -2154,7 +2163,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -2174,7 +2183,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -2194,7 +2203,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -2214,7 +2223,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -2234,7 +2243,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -2254,7 +2263,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>73</v>
       </c>
@@ -2274,7 +2283,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>74</v>
       </c>
@@ -2294,7 +2303,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -2314,7 +2323,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>76</v>
       </c>
@@ -2334,7 +2343,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -2354,7 +2363,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -2374,7 +2383,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>79</v>
       </c>
@@ -2394,7 +2403,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -2414,7 +2423,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>81</v>
       </c>
@@ -2434,7 +2443,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>82</v>
       </c>
@@ -2454,7 +2463,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>83</v>
       </c>
@@ -2474,7 +2483,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>84</v>
       </c>
@@ -2494,7 +2503,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -2514,7 +2523,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>86</v>
       </c>
@@ -2534,7 +2543,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -2554,7 +2563,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>88</v>
       </c>
@@ -2574,7 +2583,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>89</v>
       </c>
@@ -2594,7 +2603,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>90</v>
       </c>
@@ -2614,7 +2623,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -2634,7 +2643,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>92</v>
       </c>
@@ -2654,7 +2663,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -2674,7 +2683,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>94</v>
       </c>
@@ -2694,7 +2703,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -2714,7 +2723,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>96</v>
       </c>
@@ -2734,7 +2743,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>97</v>
       </c>
@@ -2754,7 +2763,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>98</v>
       </c>
@@ -2774,7 +2783,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>99</v>
       </c>
@@ -2794,7 +2803,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>100</v>
       </c>
@@ -2814,7 +2823,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>101</v>
       </c>
@@ -2834,7 +2843,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>102</v>
       </c>
@@ -2854,7 +2863,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>103</v>
       </c>
@@ -2874,7 +2883,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>104</v>
       </c>
@@ -2894,7 +2903,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>105</v>
       </c>
@@ -2914,7 +2923,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>106</v>
       </c>
@@ -2934,7 +2943,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>107</v>
       </c>
@@ -2954,7 +2963,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>108</v>
       </c>
@@ -2974,7 +2983,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>109</v>
       </c>
@@ -2994,7 +3003,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>110</v>
       </c>
@@ -3014,7 +3023,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>111</v>
       </c>
@@ -3034,7 +3043,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>112</v>
       </c>
@@ -3054,7 +3063,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>113</v>
       </c>
@@ -3074,7 +3083,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>114</v>
       </c>
@@ -3094,7 +3103,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>115</v>
       </c>
@@ -3114,7 +3123,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>116</v>
       </c>
@@ -3134,7 +3143,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>117</v>
       </c>
@@ -3154,7 +3163,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>118</v>
       </c>
@@ -3174,7 +3183,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>119</v>
       </c>
@@ -3194,7 +3203,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>120</v>
       </c>
@@ -3214,7 +3223,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>121</v>
       </c>
@@ -3234,7 +3243,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>122</v>
       </c>
@@ -3254,7 +3263,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>123</v>
       </c>
@@ -3274,7 +3283,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>124</v>
       </c>
@@ -3294,7 +3303,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>125</v>
       </c>
@@ -3314,7 +3323,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>126</v>
       </c>
@@ -3334,7 +3343,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>127</v>
       </c>
@@ -3354,7 +3363,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>128</v>
       </c>
@@ -3374,7 +3383,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>129</v>
       </c>
@@ -3394,7 +3403,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>130</v>
       </c>
@@ -3414,7 +3423,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>131</v>
       </c>
@@ -3434,7 +3443,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>132</v>
       </c>
@@ -3454,7 +3463,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>133</v>
       </c>
@@ -3474,7 +3483,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>134</v>
       </c>
@@ -3494,7 +3503,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>135</v>
       </c>
@@ -3514,7 +3523,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>136</v>
       </c>
@@ -3534,7 +3543,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>137</v>
       </c>
@@ -3554,7 +3563,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>138</v>
       </c>
@@ -3574,7 +3583,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>139</v>
       </c>
@@ -3594,7 +3603,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>140</v>
       </c>
@@ -3614,7 +3623,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>141</v>
       </c>
@@ -3634,7 +3643,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>142</v>
       </c>
@@ -3654,7 +3663,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>143</v>
       </c>
@@ -3674,7 +3683,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>144</v>
       </c>
@@ -3694,7 +3703,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>145</v>
       </c>
@@ -3714,7 +3723,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>146</v>
       </c>
@@ -3734,7 +3743,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>147</v>
       </c>
@@ -3754,7 +3763,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>148</v>
       </c>
@@ -3774,7 +3783,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>149</v>
       </c>
@@ -3794,7 +3803,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>150</v>
       </c>
@@ -3814,7 +3823,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>151</v>
       </c>
@@ -3834,7 +3843,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>152</v>
       </c>
@@ -3854,7 +3863,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>153</v>
       </c>
@@ -3874,7 +3883,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>154</v>
       </c>
@@ -3900,14 +3909,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5CB098-B380-4EF7-9313-0F60F425FD8F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0651FED3-0268-49FD-9145-9D8F0019609D}">
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>158</v>
       </c>
@@ -3915,7 +3924,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3926,7 +3935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3937,7 +3946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3948,7 +3957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3959,7 +3968,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3970,7 +3979,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3981,7 +3990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3992,7 +4001,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -4003,7 +4012,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -4014,7 +4023,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -4025,7 +4034,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -4036,7 +4045,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -4047,7 +4056,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -4058,7 +4067,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -4069,7 +4078,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -4080,7 +4089,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -4091,7 +4100,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -4102,7 +4111,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -4113,7 +4122,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -4124,7 +4133,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -4135,7 +4144,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -4146,7 +4155,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -4157,7 +4166,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -4168,7 +4177,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -4179,7 +4188,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -4190,7 +4199,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -4201,7 +4210,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -4212,7 +4221,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -4223,7 +4232,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -4234,7 +4243,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -4245,7 +4254,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -4256,7 +4265,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -4267,7 +4276,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -4278,7 +4287,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -4289,7 +4298,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -4300,7 +4309,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -4311,7 +4320,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -4322,7 +4331,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -4333,7 +4342,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -4344,7 +4353,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -4355,7 +4364,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -4366,7 +4375,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -4377,7 +4386,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -4388,7 +4397,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -4399,7 +4408,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -4410,7 +4419,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -4421,7 +4430,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -4432,7 +4441,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -4443,7 +4452,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -4454,7 +4463,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>54</v>
       </c>

</xml_diff>